<commit_message>
Extend NAO, PDO and AMO analysis
</commit_message>
<xml_diff>
--- a/charts_and_tables/NAO/phases/4 months period/Negative phases - 3 months running mean - 0.4 threshold.xlsx
+++ b/charts_and_tables/NAO/phases/4 months period/Negative phases - 3 months running mean - 0.4 threshold.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
-    <t># of La Nina</t>
+    <t># of negative phase</t>
   </si>
   <si>
     <t>Starting date</t>
@@ -25,7 +25,7 @@
     <t>Ending date</t>
   </si>
   <si>
-    <t>Months since the end of last La Nina episode</t>
+    <t>Months since the end of last negative phase episode</t>
   </si>
   <si>
     <t>Duration of episode in months</t>

</xml_diff>